<commit_message>
Modified on MAY 2 with change password
</commit_message>
<xml_diff>
--- a/Excel/changepassword.xlsx
+++ b/Excel/changepassword.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14130" windowHeight="2700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14130" windowHeight="2700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Old password</t>
   </si>
@@ -130,6 +130,36 @@
   </si>
   <si>
     <t>NEP140675</t>
+  </si>
+  <si>
+    <t>Already Email</t>
+  </si>
+  <si>
+    <t>Srivijayaragavan30@gmail.com</t>
+  </si>
+  <si>
+    <t>@gmail.com</t>
+  </si>
+  <si>
+    <t>abc@.com</t>
+  </si>
+  <si>
+    <t>abc@gmail</t>
+  </si>
+  <si>
+    <t>abced</t>
+  </si>
+  <si>
+    <t>@$%&amp;@.com</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>abcdef</t>
+  </si>
+  <si>
+    <t>abcdefg</t>
   </si>
 </sst>
 </file>
@@ -204,15 +234,18 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -510,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -519,6 +552,7 @@
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -531,6 +565,9 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="2" t="s">
@@ -543,12 +580,9 @@
         <v>3</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="E2" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -558,14 +592,53 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="E4" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="E5" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="E7" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="9" spans="1:18">
       <c r="B9">
         <v>113977</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -573,21 +646,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="8"/>
       <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
@@ -599,14 +672,14 @@
       </c>
     </row>
     <row r="2" spans="1:25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="B2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="8"/>
       <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
@@ -655,7 +728,7 @@
       <c r="X5" t="s">
         <v>16</v>
       </c>
-      <c r="Y5" s="5" t="s">
+      <c r="Y5" s="4" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>